<commit_message>
Linking settings tab to selection tab
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B555BB6E-6CFF-4373-B488-29A0AD85B418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1404BA23-D8A2-4886-9752-EF7DD002CCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="exiobase" sheetId="1" r:id="rId1"/>
-    <sheet name="german" sheetId="2" r:id="rId2"/>
-    <sheet name="english" sheetId="3" r:id="rId3"/>
+    <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
+    <sheet name="Deutsch" sheetId="2" r:id="rId2"/>
+    <sheet name="English" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,8 +719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added general dict to ui
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1404BA23-D8A2-4886-9752-EF7DD002CCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2484CCB7-B1EC-4D70-A574-07D48C5C7222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
   <si>
     <t>exiobase</t>
   </si>
@@ -104,6 +104,48 @@
   <si>
     <t>Rohstoff-
 gewinnung</t>
+  </si>
+  <si>
+    <t>Selection</t>
+  </si>
+  <si>
+    <t>Auswahl</t>
+  </si>
+  <si>
+    <t>Visualisation</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Visualisierung</t>
+  </si>
+  <si>
+    <t>Einstellungen</t>
+  </si>
+  <si>
+    <t>General Settings</t>
+  </si>
+  <si>
+    <t>Grundeinstellungen</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Sprache</t>
+  </si>
+  <si>
+    <t>Jahr</t>
+  </si>
+  <si>
+    <t>Show Indices</t>
+  </si>
+  <si>
+    <t>Indices anzeigen</t>
   </si>
 </sst>
 </file>
@@ -147,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,11 +212,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -186,6 +239,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -488,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,6 +649,62 @@
         <v>20</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -602,10 +712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +820,62 @@
         <v>15</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -717,10 +883,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="B23" sqref="A20:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +991,94 @@
         <v>21</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added full translation to all tabs and config data
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2484CCB7-B1EC-4D70-A574-07D48C5C7222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9E3B48-4A10-4F15-9965-96681AA17653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="84">
   <si>
     <t>exiobase</t>
   </si>
@@ -146,6 +146,138 @@
   </si>
   <si>
     <t>Indices anzeigen</t>
+  </si>
+  <si>
+    <t>Region Selection</t>
+  </si>
+  <si>
+    <t>Region-Auswahl</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>Lösche</t>
+  </si>
+  <si>
+    <t>Select All Regions</t>
+  </si>
+  <si>
+    <t>Wähle alle Regionen aus</t>
+  </si>
+  <si>
+    <t>Sector Selection</t>
+  </si>
+  <si>
+    <t>Select All Sectors</t>
+  </si>
+  <si>
+    <t>Sektor-Auswahl</t>
+  </si>
+  <si>
+    <t>Wähle alle Sektoren aus</t>
+  </si>
+  <si>
+    <t>Selection Summary</t>
+  </si>
+  <si>
+    <t>Zusammenfassung der Auswahl</t>
+  </si>
+  <si>
+    <t>No selection made</t>
+  </si>
+  <si>
+    <t>Keine Auswahl getroffen</t>
+  </si>
+  <si>
+    <t>Apply Selection</t>
+  </si>
+  <si>
+    <t>Aktuelle Auswahl übernehmen</t>
+  </si>
+  <si>
+    <t>Reset All Selections</t>
+  </si>
+  <si>
+    <t>Alles zurücksetzen</t>
+  </si>
+  <si>
+    <t>Regions</t>
+  </si>
+  <si>
+    <t>Regionen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sectors </t>
+  </si>
+  <si>
+    <t>Sektoren</t>
+  </si>
+  <si>
+    <t>No regions selected</t>
+  </si>
+  <si>
+    <t>No sectors selected</t>
+  </si>
+  <si>
+    <t>Keine Regionen ausgewählt</t>
+  </si>
+  <si>
+    <t>Keine Sektoren ausgewählt</t>
+  </si>
+  <si>
+    <t>All regions selected (Global view)</t>
+  </si>
+  <si>
+    <t>All sectors selected (Global view)</t>
+  </si>
+  <si>
+    <t>Alle Regionen ausgewählt (Globale Ansicht)</t>
+  </si>
+  <si>
+    <t>Alle Sektoren ausgewählt (Globale Ansicht)</t>
+  </si>
+  <si>
+    <t>Sector indices count</t>
+  </si>
+  <si>
+    <t>Anzahl der Sektoren</t>
+  </si>
+  <si>
+    <t>Region indices count</t>
+  </si>
+  <si>
+    <t>Anzahl der Regionen</t>
+  </si>
+  <si>
+    <t>World Map</t>
+  </si>
+  <si>
+    <t>Weltkarte</t>
+  </si>
+  <si>
+    <t>Select Impacts</t>
+  </si>
+  <si>
+    <t>Wähle Umweltindikatoren</t>
+  </si>
+  <si>
+    <t>Selected</t>
+  </si>
+  <si>
+    <t>Ausgewählt</t>
+  </si>
+  <si>
+    <t>Update Plot</t>
+  </si>
+  <si>
+    <t>Plot aktualisieren</t>
+  </si>
+  <si>
+    <t>Reset to Defaults</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zurücksetzen </t>
   </si>
 </sst>
 </file>
@@ -227,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -239,7 +371,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -542,15 +675,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,59 +783,235 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -712,16 +1021,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -808,7 +1117,7 @@
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -821,78 +1130,254 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="2" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="A20:B23"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B45" sqref="A41:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -992,91 +1477,267 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added title to supply chain analysis
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA837A77-4C53-49D4-BEF2-ADE63D3E2BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0A9C63-810D-419F-9365-F91D93A0B7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="88">
   <si>
     <t>exiobase</t>
   </si>
@@ -278,6 +278,18 @@
   </si>
   <si>
     <t>Sectors</t>
+  </si>
+  <si>
+    <t>of a</t>
+  </si>
+  <si>
+    <t>einer</t>
+  </si>
+  <si>
+    <t>spezifischen Auswahl von Sektoren</t>
+  </si>
+  <si>
+    <t>specific selection of sectors</t>
   </si>
 </sst>
 </file>
@@ -359,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -372,6 +384,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -674,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,6 +1026,22 @@
         <v>81</v>
       </c>
     </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1020,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B43" sqref="A42:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,6 +1389,22 @@
         <v>82</v>
       </c>
     </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1368,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,6 +1784,22 @@
         <v>81</v>
       </c>
     </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed language switch for the settings tab
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F100EDE7-C73E-43CE-A4B7-6CC523F10940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271EFA71-72EC-4AEC-8E71-98DABE6CB7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="93">
   <si>
     <t>exiobase</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>world</t>
+  </si>
+  <si>
+    <t>Optionen</t>
   </si>
 </sst>
 </file>
@@ -1581,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2112,12 +2115,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -2611,7 +2616,7 @@
         <v>46</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="5"/>

</xml_diff>

<commit_message>
New impact matrices, divided in regional impacts
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17308410-2E67-4E5F-8BEC-2A8644A87513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723CC9E3-D999-48CF-886D-7C531E4D789C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="105">
   <si>
     <t>exiobase</t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>mehr Input benötigt</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Globale/r/s</t>
   </si>
 </sst>
 </file>
@@ -380,7 +386,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -390,46 +396,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -437,18 +413,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1612,564 +1587,434 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="4" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="2" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2183,564 +2028,434 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView showGridLines="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="2" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2754,608 +2469,466 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:B55"/>
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" style="4" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    </row>
+    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-    </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-    </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="4"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-    </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+    </row>
+    <row r="49" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="4"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-    </row>
-    <row r="50" spans="1:5" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="4"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+    <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+    <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+    <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="2" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor Changes to general.xlsx (translations)
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A089F5-E02F-424B-94F4-4CB0E893B7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4725C90C-6A53-4ED4-8F94-7228F83DCF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="111">
   <si>
     <t>exiobase</t>
   </si>
@@ -353,6 +353,12 @@
   </si>
   <si>
     <t>Bitte aktualisieren</t>
+  </si>
+  <si>
+    <t>of the World</t>
+  </si>
+  <si>
+    <t>der Welt</t>
   </si>
 </sst>
 </file>
@@ -1606,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:B54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2052,6 +2058,14 @@
         <v>107</v>
       </c>
     </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -2063,10 +2077,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B54" sqref="A53:B54"/>
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2509,6 +2523,14 @@
         <v>108</v>
       </c>
     </row>
+    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -2520,10 +2542,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2998,6 +3020,14 @@
         <v>107</v>
       </c>
     </row>
+    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Minor design changes to the ToolTip Dialog
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11678D8E-9851-4A40-90D9-C507DEC13C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D29FAC-731B-4E6C-85DA-838427FF63F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="121">
   <si>
     <t>exiobase</t>
   </si>
@@ -377,6 +377,18 @@
   </si>
   <si>
     <t>Plot abspeichern</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Prozentwert</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Info</t>
   </si>
 </sst>
 </file>
@@ -1630,10 +1642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:B58"/>
+    <sheetView showGridLines="0" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2108,6 +2120,30 @@
         <v>114</v>
       </c>
     </row>
+    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -2119,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B58"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView showGridLines="0" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2597,6 +2633,30 @@
         <v>115</v>
       </c>
     </row>
+    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -2608,10 +2668,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3118,6 +3178,30 @@
         <v>114</v>
       </c>
     </row>
+    <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
New plot worldmap function
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296C6D6A-3466-4163-976C-5BEDE8FC27B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECBB5E2-663F-4FB1-8F35-A0D3063AA90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Farbe</t>
   </si>
   <si>
-    <t>Einzelhandel</t>
-  </si>
-  <si>
     <t>Direkte
 Zulieferer</t>
   </si>
@@ -431,6 +428,10 @@
   </si>
   <si>
     <t>Dunkelmodus</t>
+  </si>
+  <si>
+    <t>Konsumgüter-
+produktion</t>
   </si>
 </sst>
 </file>
@@ -1699,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2080,130 +2081,130 @@
     </row>
     <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
@@ -2216,50 +2217,50 @@
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2275,8 +2276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B68"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2327,12 +2328,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
+      <c r="B6" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2340,7 +2341,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2348,7 +2349,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2356,7 +2357,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2364,7 +2365,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2372,7 +2373,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2380,7 +2381,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2388,7 +2389,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2396,7 +2397,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2404,7 +2405,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2412,7 +2413,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2420,7 +2421,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2429,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2436,7 +2437,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2444,7 +2445,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2452,7 +2453,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2460,7 +2461,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2468,7 +2469,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2476,7 +2477,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2484,7 +2485,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2492,7 +2493,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2500,7 +2501,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2508,7 +2509,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2516,7 +2517,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2524,7 +2525,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,7 +2533,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2540,7 +2541,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2548,7 +2549,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2556,7 +2557,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2564,7 +2565,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2572,7 +2573,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2580,7 +2581,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2588,7 +2589,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2596,7 +2597,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2604,7 +2605,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2612,7 +2613,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2620,7 +2621,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2628,7 +2629,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2644,7 +2645,7 @@
         <v>46</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -2652,183 +2653,183 @@
         <v>19</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>125</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B65" t="s">
         <v>127</v>
-      </c>
-      <c r="B65" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B68" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2941,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2948,7 +2949,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3012,7 +3013,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3020,7 +3021,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3028,7 +3029,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3036,7 +3037,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3257,178 +3258,178 @@
     </row>
     <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More color themes for maps
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5DF2C5-97F7-4D21-99D3-3D08D80895D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC617368-1C34-4EE6-93D3-C04F831CE6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="337">
   <si>
     <t>exiobase</t>
   </si>
@@ -540,17 +540,522 @@
   </si>
   <si>
     <t>Stage Analysis</t>
+  </si>
+  <si>
+    <t>Region Analysis</t>
+  </si>
+  <si>
+    <t>Analyse nach Wertschöpfungsstufen</t>
+  </si>
+  <si>
+    <t>Analyse nach Regionen</t>
+  </si>
+  <si>
+    <t>World Map Settings</t>
+  </si>
+  <si>
+    <t>Erweiterte Einstellungen</t>
+  </si>
+  <si>
+    <t>Farbkarte</t>
+  </si>
+  <si>
+    <t>cm.group.perceptual</t>
+  </si>
+  <si>
+    <t>Perzeptuell</t>
+  </si>
+  <si>
+    <t>cm.group.sequential</t>
+  </si>
+  <si>
+    <t>Sequenziell</t>
+  </si>
+  <si>
+    <t>cm.group.diverging</t>
+  </si>
+  <si>
+    <t>Divergierend</t>
+  </si>
+  <si>
+    <t>cm.group.cyclic</t>
+  </si>
+  <si>
+    <t>Zyklisch</t>
+  </si>
+  <si>
+    <t>cm.group.qualitative</t>
+  </si>
+  <si>
+    <t>Qualitativ</t>
+  </si>
+  <si>
+    <t>cm.reverse</t>
+  </si>
+  <si>
+    <t>Umkehren</t>
+  </si>
+  <si>
+    <t>cmap.Reds</t>
+  </si>
+  <si>
+    <t>Rottöne</t>
+  </si>
+  <si>
+    <t>cmap.Blues</t>
+  </si>
+  <si>
+    <t>Blautöne</t>
+  </si>
+  <si>
+    <t>cmap.Greens</t>
+  </si>
+  <si>
+    <t>Grüntöne</t>
+  </si>
+  <si>
+    <t>cmap.Purples</t>
+  </si>
+  <si>
+    <t>Violettöne</t>
+  </si>
+  <si>
+    <t>cmap.Oranges</t>
+  </si>
+  <si>
+    <t>Orangetöne</t>
+  </si>
+  <si>
+    <t>cmap.Greys</t>
+  </si>
+  <si>
+    <t>Grautöne</t>
+  </si>
+  <si>
+    <t>cmap.YlGn</t>
+  </si>
+  <si>
+    <t>Gelb–Grün</t>
+  </si>
+  <si>
+    <t>cmap.YlGnBu</t>
+  </si>
+  <si>
+    <t>Gelb–Grün–Blau</t>
+  </si>
+  <si>
+    <t>cmap.GnBu</t>
+  </si>
+  <si>
+    <t>Grün–Blau</t>
+  </si>
+  <si>
+    <t>cmap.BuGn</t>
+  </si>
+  <si>
+    <t>Blau–Grün</t>
+  </si>
+  <si>
+    <t>cmap.PuBu</t>
+  </si>
+  <si>
+    <t>Violett–Blau</t>
+  </si>
+  <si>
+    <t>cmap.BuPu</t>
+  </si>
+  <si>
+    <t>Blau–Violett</t>
+  </si>
+  <si>
+    <t>cmap.OrRd</t>
+  </si>
+  <si>
+    <t>Orange–Rot</t>
+  </si>
+  <si>
+    <t>cmap.PuRd</t>
+  </si>
+  <si>
+    <t>Violett–Rot</t>
+  </si>
+  <si>
+    <t>cmap.RdPu</t>
+  </si>
+  <si>
+    <t>Rot–Violett</t>
+  </si>
+  <si>
+    <t>cmap.YlOrBr</t>
+  </si>
+  <si>
+    <t>Gelb–Orange–Braun</t>
+  </si>
+  <si>
+    <t>cmap.YlOrRd</t>
+  </si>
+  <si>
+    <t>Gelb–Orange–Rot</t>
+  </si>
+  <si>
+    <t>cmap.viridis</t>
+  </si>
+  <si>
+    <t>Viridis</t>
+  </si>
+  <si>
+    <t>cmap.plasma</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>cmap.inferno</t>
+  </si>
+  <si>
+    <t>Inferno</t>
+  </si>
+  <si>
+    <t>cmap.magma</t>
+  </si>
+  <si>
+    <t>Magma</t>
+  </si>
+  <si>
+    <t>cmap.cividis</t>
+  </si>
+  <si>
+    <t>Cividis</t>
+  </si>
+  <si>
+    <t>cmap.turbo</t>
+  </si>
+  <si>
+    <t>Turbo</t>
+  </si>
+  <si>
+    <t>cmap.BrBG</t>
+  </si>
+  <si>
+    <t>Braun–Blaugrün</t>
+  </si>
+  <si>
+    <t>cmap.PiYG</t>
+  </si>
+  <si>
+    <t>Pink–Gelbgrün</t>
+  </si>
+  <si>
+    <t>cmap.PRGn</t>
+  </si>
+  <si>
+    <t>Purpur–Grün</t>
+  </si>
+  <si>
+    <t>cmap.PuOr</t>
+  </si>
+  <si>
+    <t>Violett–Orange</t>
+  </si>
+  <si>
+    <t>cmap.RdBu</t>
+  </si>
+  <si>
+    <t>Rot–Blau</t>
+  </si>
+  <si>
+    <t>cmap.RdGy</t>
+  </si>
+  <si>
+    <t>Rot–Grau</t>
+  </si>
+  <si>
+    <t>cmap.RdYlBu</t>
+  </si>
+  <si>
+    <t>Rot–Gelb–Blau</t>
+  </si>
+  <si>
+    <t>cmap.RdYlGn</t>
+  </si>
+  <si>
+    <t>Rot–Gelb–Grün</t>
+  </si>
+  <si>
+    <t>cmap.Spectral</t>
+  </si>
+  <si>
+    <t>Spektral</t>
+  </si>
+  <si>
+    <t>cmap.coolwarm</t>
+  </si>
+  <si>
+    <t>Cool–Warm</t>
+  </si>
+  <si>
+    <t>cmap.bwr</t>
+  </si>
+  <si>
+    <t>Blau–Weiß–Rot</t>
+  </si>
+  <si>
+    <t>cmap.seismic</t>
+  </si>
+  <si>
+    <t>Seismisch</t>
+  </si>
+  <si>
+    <t>cmap.twilight</t>
+  </si>
+  <si>
+    <t>Twilight</t>
+  </si>
+  <si>
+    <t>cmap.twilight_shifted</t>
+  </si>
+  <si>
+    <t>Twilight (verschoben)</t>
+  </si>
+  <si>
+    <t>cmap.hsv</t>
+  </si>
+  <si>
+    <t>HSV</t>
+  </si>
+  <si>
+    <t>cmap.tab10</t>
+  </si>
+  <si>
+    <t>Tab10</t>
+  </si>
+  <si>
+    <t>cmap.tab20</t>
+  </si>
+  <si>
+    <t>Tab20</t>
+  </si>
+  <si>
+    <t>cmap.tab20b</t>
+  </si>
+  <si>
+    <t>Tab20b</t>
+  </si>
+  <si>
+    <t>cmap.tab20c</t>
+  </si>
+  <si>
+    <t>Tab20c</t>
+  </si>
+  <si>
+    <t>cmap.Set1</t>
+  </si>
+  <si>
+    <t>Set1</t>
+  </si>
+  <si>
+    <t>cmap.Set2</t>
+  </si>
+  <si>
+    <t>Set2</t>
+  </si>
+  <si>
+    <t>cmap.Set3</t>
+  </si>
+  <si>
+    <t>Set3</t>
+  </si>
+  <si>
+    <t>cmap.Pastel1</t>
+  </si>
+  <si>
+    <t>Pastel1</t>
+  </si>
+  <si>
+    <t>cmap.Pastel2</t>
+  </si>
+  <si>
+    <t>Pastel2</t>
+  </si>
+  <si>
+    <t>cmap.Accent</t>
+  </si>
+  <si>
+    <t>Accent</t>
+  </si>
+  <si>
+    <t>cmap.Dark2</t>
+  </si>
+  <si>
+    <t>Dark2</t>
+  </si>
+  <si>
+    <t>cmap.Paired</t>
+  </si>
+  <si>
+    <t>Paired</t>
+  </si>
+  <si>
+    <t>Perceptual</t>
+  </si>
+  <si>
+    <t>Sequential</t>
+  </si>
+  <si>
+    <t>Diverging</t>
+  </si>
+  <si>
+    <t>Cyclic</t>
+  </si>
+  <si>
+    <t>Qualitative</t>
+  </si>
+  <si>
+    <t>Reverse</t>
+  </si>
+  <si>
+    <t>Reds</t>
+  </si>
+  <si>
+    <t>Blues</t>
+  </si>
+  <si>
+    <t>Greens</t>
+  </si>
+  <si>
+    <t>Purples</t>
+  </si>
+  <si>
+    <t>Oranges</t>
+  </si>
+  <si>
+    <t>Greys</t>
+  </si>
+  <si>
+    <t>YlGn</t>
+  </si>
+  <si>
+    <t>YlGnBu</t>
+  </si>
+  <si>
+    <t>GnBu</t>
+  </si>
+  <si>
+    <t>BuGn</t>
+  </si>
+  <si>
+    <t>PuBu</t>
+  </si>
+  <si>
+    <t>BuPu</t>
+  </si>
+  <si>
+    <t>OrRd</t>
+  </si>
+  <si>
+    <t>PuRd</t>
+  </si>
+  <si>
+    <t>RdPu</t>
+  </si>
+  <si>
+    <t>YlOrBr</t>
+  </si>
+  <si>
+    <t>YlOrRd</t>
+  </si>
+  <si>
+    <t>viridis</t>
+  </si>
+  <si>
+    <t>plasma</t>
+  </si>
+  <si>
+    <t>inferno</t>
+  </si>
+  <si>
+    <t>magma</t>
+  </si>
+  <si>
+    <t>cividis</t>
+  </si>
+  <si>
+    <t>turbo</t>
+  </si>
+  <si>
+    <t>BrBG</t>
+  </si>
+  <si>
+    <t>PiYG</t>
+  </si>
+  <si>
+    <t>PRGn</t>
+  </si>
+  <si>
+    <t>PuOr</t>
+  </si>
+  <si>
+    <t>RdBu</t>
+  </si>
+  <si>
+    <t>RdGy</t>
+  </si>
+  <si>
+    <t>RdYlBu</t>
+  </si>
+  <si>
+    <t>RdYlGn</t>
+  </si>
+  <si>
+    <t>Spectral</t>
+  </si>
+  <si>
+    <t>coolwarm</t>
+  </si>
+  <si>
+    <t>bwr</t>
+  </si>
+  <si>
+    <t>seismic</t>
+  </si>
+  <si>
+    <t>twilight</t>
+  </si>
+  <si>
+    <t>twilight_shifted</t>
+  </si>
+  <si>
+    <t>hsv</t>
+  </si>
+  <si>
+    <t>tab10</t>
+  </si>
+  <si>
+    <t>tab20</t>
+  </si>
+  <si>
+    <t>tab20b</t>
+  </si>
+  <si>
+    <t>tab20c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -574,6 +1079,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -626,29 +1137,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{C2F78208-F7F8-4542-9E5B-6270DCB86735}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1806,20 +2320,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85:B88"/>
+    <sheetView showGridLines="0" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="115" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" style="4" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1835,7 +2350,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13.5" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1843,7 +2358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1851,7 +2366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1859,7 +2374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1867,7 +2382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1875,7 +2390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1883,7 +2398,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1891,7 +2406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="13.5" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1899,7 +2414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13.5" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1907,7 +2422,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13.5" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -1915,7 +2430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1923,7 +2438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1931,7 +2446,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1939,7 +2454,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="13.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1947,7 +2462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="13.5" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1955,7 +2470,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="13.5" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1963,7 +2478,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1971,7 +2486,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1979,7 +2494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="13.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1987,7 +2502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1995,7 +2510,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13.5" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -2003,7 +2518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="13.5" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -2011,7 +2526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -2019,7 +2534,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="13.5" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2027,7 +2542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -2035,7 +2550,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.5" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2043,7 +2558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -2051,7 +2566,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="13.5" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -2059,7 +2574,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -2067,7 +2582,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="13.5" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -2075,7 +2590,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -2083,7 +2598,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="13.5" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -2091,7 +2606,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="13.5" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -2099,7 +2614,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -2107,7 +2622,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -2115,7 +2630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -2123,7 +2638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -2131,7 +2646,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -2139,7 +2654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="13.5" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -2147,7 +2662,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -2155,7 +2670,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -2163,7 +2678,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.95" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -2171,7 +2686,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.95" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2179,7 +2694,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>19</v>
       </c>
@@ -2187,7 +2702,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2195,7 +2710,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2203,7 +2718,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2211,7 +2726,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2219,7 +2734,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2227,7 +2742,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>102</v>
       </c>
@@ -2235,7 +2750,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>104</v>
       </c>
@@ -2243,7 +2758,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>106</v>
       </c>
@@ -2251,7 +2766,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>108</v>
       </c>
@@ -2259,7 +2774,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>110</v>
       </c>
@@ -2267,7 +2782,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>112</v>
       </c>
@@ -2275,7 +2790,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>113</v>
       </c>
@@ -2283,7 +2798,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>118</v>
       </c>
@@ -2291,7 +2806,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>116</v>
       </c>
@@ -2299,7 +2814,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>117</v>
       </c>
@@ -2307,7 +2822,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>120</v>
       </c>
@@ -2323,7 +2838,7 @@
       <c r="I62" s="8"/>
       <c r="J62" s="8"/>
     </row>
-    <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>122</v>
       </c>
@@ -2331,7 +2846,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15" customHeight="1">
       <c r="A64" s="7" t="s">
         <v>124</v>
       </c>
@@ -2339,7 +2854,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="15" customHeight="1">
       <c r="A65" s="9" t="s">
         <v>126</v>
       </c>
@@ -2347,7 +2862,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="15" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>129</v>
       </c>
@@ -2355,7 +2870,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="15" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>130</v>
       </c>
@@ -2363,7 +2878,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="15" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>132</v>
       </c>
@@ -2371,7 +2886,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="15" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>135</v>
       </c>
@@ -2379,7 +2894,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="15" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>137</v>
       </c>
@@ -2387,7 +2902,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="15" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>138</v>
       </c>
@@ -2395,7 +2910,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="15" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>139</v>
       </c>
@@ -2403,7 +2918,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="15" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>140</v>
       </c>
@@ -2411,7 +2926,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="15" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>141</v>
       </c>
@@ -2419,7 +2934,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>142</v>
       </c>
@@ -2427,7 +2942,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="15" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>143</v>
       </c>
@@ -2435,7 +2950,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="15" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>144</v>
       </c>
@@ -2443,7 +2958,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="15" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>145</v>
       </c>
@@ -2451,7 +2966,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="15" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>146</v>
       </c>
@@ -2459,7 +2974,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="15" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>147</v>
       </c>
@@ -2467,7 +2982,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>148</v>
       </c>
@@ -2475,7 +2990,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="15" customHeight="1">
       <c r="A82" s="4" t="s">
         <v>149</v>
       </c>
@@ -2483,7 +2998,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="15" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>150</v>
       </c>
@@ -2491,7 +3006,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="15" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>151</v>
       </c>
@@ -2499,7 +3014,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>162</v>
       </c>
@@ -2507,7 +3022,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>163</v>
       </c>
@@ -2515,7 +3030,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="15" customHeight="1">
       <c r="A87" s="4" t="s">
         <v>164</v>
       </c>
@@ -2523,12 +3038,492 @@
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="15" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B88" s="4" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15" customHeight="1">
+      <c r="A89" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" customHeight="1">
+      <c r="A90" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" customHeight="1">
+      <c r="A91" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" customHeight="1">
+      <c r="A92" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" customHeight="1">
+      <c r="A93" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" customHeight="1">
+      <c r="A94" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" customHeight="1">
+      <c r="A95" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" customHeight="1">
+      <c r="A96" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" customHeight="1">
+      <c r="A97" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" customHeight="1">
+      <c r="A98" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15" customHeight="1">
+      <c r="A99" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" customHeight="1">
+      <c r="A100" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" customHeight="1">
+      <c r="A101" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15" customHeight="1">
+      <c r="A102" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15" customHeight="1">
+      <c r="A103" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" customHeight="1">
+      <c r="A104" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" customHeight="1">
+      <c r="A105" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15" customHeight="1">
+      <c r="A106" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" customHeight="1">
+      <c r="A107" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15" customHeight="1">
+      <c r="A108" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15" customHeight="1">
+      <c r="A109" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" customHeight="1">
+      <c r="A110" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15" customHeight="1">
+      <c r="A111" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" customHeight="1">
+      <c r="A112" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15" customHeight="1">
+      <c r="A113" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15" customHeight="1">
+      <c r="A114" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" customHeight="1">
+      <c r="A115" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" customHeight="1">
+      <c r="A116" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" customHeight="1">
+      <c r="A117" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15" customHeight="1">
+      <c r="A118" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15" customHeight="1">
+      <c r="A119" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15" customHeight="1">
+      <c r="A120" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15" customHeight="1">
+      <c r="A121" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15" customHeight="1">
+      <c r="A122" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15" customHeight="1">
+      <c r="A123" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15" customHeight="1">
+      <c r="A124" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15" customHeight="1">
+      <c r="A125" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15" customHeight="1">
+      <c r="A126" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15" customHeight="1">
+      <c r="A127" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15" customHeight="1">
+      <c r="A128" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15" customHeight="1">
+      <c r="A129" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15" customHeight="1">
+      <c r="A130" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" customHeight="1">
+      <c r="A131" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" customHeight="1">
+      <c r="A132" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" customHeight="1">
+      <c r="A133" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15" customHeight="1">
+      <c r="A134" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15" customHeight="1">
+      <c r="A135" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" customHeight="1">
+      <c r="A136" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15" customHeight="1">
+      <c r="A137" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15" customHeight="1">
+      <c r="A138" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" customHeight="1">
+      <c r="A139" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" customHeight="1">
+      <c r="A140" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15" customHeight="1">
+      <c r="A141" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" customHeight="1">
+      <c r="A142" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" customHeight="1">
+      <c r="A143" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" customHeight="1">
+      <c r="A144" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" customHeight="1">
+      <c r="A145" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15" customHeight="1">
+      <c r="A146" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15" customHeight="1">
+      <c r="A147" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15" customHeight="1">
+      <c r="A148" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2542,21 +3537,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView showGridLines="0" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="115" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75" style="4" customWidth="1"/>
+    <col min="1" max="1" width="54.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2564,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -2572,7 +3567,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13.5" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -2580,7 +3575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2588,7 +3583,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -2596,7 +3591,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="30">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2604,7 +3599,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="30" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2612,7 +3607,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="45" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2620,7 +3615,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="30" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2628,7 +3623,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="13.5" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -2636,7 +3631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13.5" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -2644,7 +3639,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13.5" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -2652,7 +3647,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -2660,7 +3655,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -2668,7 +3663,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -2676,7 +3671,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="13.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -2684,7 +3679,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="13.5" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -2692,7 +3687,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="13.5" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -2700,7 +3695,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -2708,7 +3703,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -2716,7 +3711,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="13.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -2724,7 +3719,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2732,7 +3727,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13.5" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
@@ -2740,7 +3735,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="13.5" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -2748,7 +3743,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
@@ -2756,7 +3751,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="13.5" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2764,7 +3759,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -2772,7 +3767,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.5" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>28</v>
       </c>
@@ -2780,7 +3775,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
@@ -2788,7 +3783,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="13.5" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>30</v>
       </c>
@@ -2796,7 +3791,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
@@ -2804,7 +3799,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="13.5" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
@@ -2812,7 +3807,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
@@ -2820,7 +3815,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="13.5" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -2828,7 +3823,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="13.5" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
@@ -2836,7 +3831,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
@@ -2844,7 +3839,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
@@ -2852,7 +3847,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -2860,7 +3855,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -2868,7 +3863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>40</v>
       </c>
@@ -2876,7 +3871,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="13.5" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -2884,7 +3879,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>42</v>
       </c>
@@ -2892,7 +3887,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -2900,7 +3895,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.95" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>44</v>
       </c>
@@ -2908,7 +3903,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.95" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2916,7 +3911,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="15.95" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>19</v>
       </c>
@@ -2924,7 +3919,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="15" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2932,7 +3927,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2940,7 +3935,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2948,7 +3943,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="15" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2956,7 +3951,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="15" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2964,7 +3959,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="15" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>102</v>
       </c>
@@ -2972,7 +3967,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="15" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>104</v>
       </c>
@@ -2980,7 +3975,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>106</v>
       </c>
@@ -2988,7 +3983,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>108</v>
       </c>
@@ -2996,7 +3991,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>110</v>
       </c>
@@ -3004,7 +3999,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="15" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>112</v>
       </c>
@@ -3012,7 +4007,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="15" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>113</v>
       </c>
@@ -3020,7 +4015,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>118</v>
       </c>
@@ -3028,7 +4023,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="15" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>116</v>
       </c>
@@ -3036,7 +4031,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="15" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>117</v>
       </c>
@@ -3044,7 +4039,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="15" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>120</v>
       </c>
@@ -3052,7 +4047,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="15" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>122</v>
       </c>
@@ -3060,7 +4055,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="15" customHeight="1">
       <c r="A64" s="7" t="s">
         <v>124</v>
       </c>
@@ -3068,7 +4063,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="15" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>126</v>
       </c>
@@ -3076,7 +4071,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="15" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>129</v>
       </c>
@@ -3084,7 +4079,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="15" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>130</v>
       </c>
@@ -3092,7 +4087,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="15" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>132</v>
       </c>
@@ -3100,7 +4095,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="15" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>135</v>
       </c>
@@ -3108,7 +4103,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="15" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>137</v>
       </c>
@@ -3116,7 +4111,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="15" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>138</v>
       </c>
@@ -3124,7 +4119,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="15" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>139</v>
       </c>
@@ -3132,7 +4127,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="15" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>140</v>
       </c>
@@ -3140,7 +4135,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="15" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>141</v>
       </c>
@@ -3148,7 +4143,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>142</v>
       </c>
@@ -3156,7 +4151,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="15" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>143</v>
       </c>
@@ -3164,7 +4159,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="15" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>144</v>
       </c>
@@ -3172,7 +4167,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="15" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>145</v>
       </c>
@@ -3180,7 +4175,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="15" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>146</v>
       </c>
@@ -3188,7 +4183,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="15" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>147</v>
       </c>
@@ -3196,7 +4191,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>148</v>
       </c>
@@ -3204,7 +4199,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="15" customHeight="1">
       <c r="A82" s="4" t="s">
         <v>149</v>
       </c>
@@ -3212,7 +4207,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="15" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>150</v>
       </c>
@@ -3220,7 +4215,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="15" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>151</v>
       </c>
@@ -3228,7 +4223,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>162</v>
       </c>
@@ -3236,7 +4231,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>163</v>
       </c>
@@ -3244,7 +4239,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="15" customHeight="1">
       <c r="A87" s="4" t="s">
         <v>164</v>
       </c>
@@ -3252,7 +4247,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="15" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>165</v>
       </c>
@@ -3260,14 +4255,489 @@
         <v>169</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="15" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B89" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15" customHeight="1">
+      <c r="A90" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15" customHeight="1">
+      <c r="A91" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15" customHeight="1">
+      <c r="A92" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" customHeight="1">
+      <c r="A93" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" customHeight="1">
+      <c r="A94" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" customHeight="1">
+      <c r="A95" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" customHeight="1">
+      <c r="A96" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" customHeight="1">
+      <c r="A97" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" customHeight="1">
+      <c r="A98" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15" customHeight="1">
+      <c r="A99" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" customHeight="1">
+      <c r="A100" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" customHeight="1">
+      <c r="A101" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15" customHeight="1">
+      <c r="A102" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15" customHeight="1">
+      <c r="A103" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" customHeight="1">
+      <c r="A104" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" customHeight="1">
+      <c r="A105" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15" customHeight="1">
+      <c r="A106" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" customHeight="1">
+      <c r="A107" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15" customHeight="1">
+      <c r="A108" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15" customHeight="1">
+      <c r="A109" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" customHeight="1">
+      <c r="A110" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15" customHeight="1">
+      <c r="A111" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" customHeight="1">
+      <c r="A112" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15" customHeight="1">
+      <c r="A113" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15" customHeight="1">
+      <c r="A114" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" customHeight="1">
+      <c r="A115" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" customHeight="1">
+      <c r="A116" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" customHeight="1">
+      <c r="A117" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15" customHeight="1">
+      <c r="A118" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15" customHeight="1">
+      <c r="A119" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15" customHeight="1">
+      <c r="A120" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15" customHeight="1">
+      <c r="A121" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15" customHeight="1">
+      <c r="A122" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15" customHeight="1">
+      <c r="A123" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15" customHeight="1">
+      <c r="A124" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15" customHeight="1">
+      <c r="A125" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15" customHeight="1">
+      <c r="A126" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15" customHeight="1">
+      <c r="A127" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15" customHeight="1">
+      <c r="A128" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15" customHeight="1">
+      <c r="A129" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15" customHeight="1">
+      <c r="A130" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" customHeight="1">
+      <c r="A131" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" customHeight="1">
+      <c r="A132" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" customHeight="1">
+      <c r="A133" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15" customHeight="1">
+      <c r="A134" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15" customHeight="1">
+      <c r="A135" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" customHeight="1">
+      <c r="A136" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15" customHeight="1">
+      <c r="A137" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15" customHeight="1">
+      <c r="A138" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" customHeight="1">
+      <c r="A139" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" customHeight="1">
+      <c r="A140" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15" customHeight="1">
+      <c r="A141" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" customHeight="1">
+      <c r="A142" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" customHeight="1">
+      <c r="A143" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" customHeight="1">
+      <c r="A144" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" customHeight="1">
+      <c r="A145" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15" customHeight="1">
+      <c r="A146" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15" customHeight="1">
+      <c r="A147" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15" customHeight="1">
+      <c r="A148" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>288</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -3276,20 +4746,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B152"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89:B92"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="115" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64" style="4" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="4" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="13.5" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3297,7 +4768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="13.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3305,7 +4776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="13.5" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -3313,7 +4784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="13.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3321,7 +4792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="13.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -3329,7 +4800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="13.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -3337,7 +4808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="13.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -3345,7 +4816,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="13.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -3353,7 +4824,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="13.5" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -3361,7 +4832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="13.5" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -3369,7 +4840,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="13.5" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -3377,7 +4848,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="13.5" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -3385,7 +4856,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="13.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -3393,7 +4864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="13.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -3401,7 +4872,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -3409,7 +4880,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="13.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -3417,7 +4888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="13.5" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -3425,7 +4896,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="13.5" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -3433,7 +4904,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="13.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
@@ -3441,7 +4912,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="13.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -3449,7 +4920,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="13.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3457,7 +4928,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="13.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -3465,7 +4936,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="13.5" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -3473,7 +4944,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="13.5" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -3481,7 +4952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="13.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -3489,7 +4960,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="13.5" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -3497,7 +4968,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="13.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -3505,7 +4976,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="13.5" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -3513,7 +4984,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" ht="13.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -3521,7 +4992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="13.5" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -3529,7 +5000,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" ht="13.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -3537,7 +5008,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="13.5" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -3545,7 +5016,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="13.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -3553,7 +5024,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="13.5" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -3561,7 +5032,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" ht="13.5" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
@@ -3569,7 +5040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="13.5" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
@@ -3577,7 +5048,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="13.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
@@ -3585,7 +5056,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="13.5" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
@@ -3593,7 +5064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="13.5" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
@@ -3601,7 +5072,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
@@ -3609,7 +5080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="13.5" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
@@ -3617,7 +5088,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
@@ -3625,7 +5096,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
@@ -3633,7 +5104,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="13.5" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>40</v>
       </c>
@@ -3641,7 +5112,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="13.5" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>41</v>
       </c>
@@ -3649,7 +5120,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>42</v>
       </c>
@@ -3657,7 +5128,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
@@ -3665,7 +5136,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" ht="15.95" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
@@ -3673,7 +5144,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="15.95" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>46</v>
       </c>
@@ -3681,7 +5152,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="15.95" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>19</v>
       </c>
@@ -3689,7 +5160,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="15" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>92</v>
       </c>
@@ -3697,7 +5168,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="15" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>94</v>
       </c>
@@ -3705,7 +5176,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="15" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -3713,7 +5184,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="15" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>98</v>
       </c>
@@ -3721,7 +5192,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="15" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>100</v>
       </c>
@@ -3729,7 +5200,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="15" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>102</v>
       </c>
@@ -3737,7 +5208,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="15" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>104</v>
       </c>
@@ -3745,7 +5216,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="15" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>106</v>
       </c>
@@ -3753,7 +5224,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="15" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>108</v>
       </c>
@@ -3761,7 +5232,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="15" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>110</v>
       </c>
@@ -3769,7 +5240,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="15" customHeight="1">
       <c r="A61" s="4" t="s">
         <v>112</v>
       </c>
@@ -3777,7 +5248,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="15" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>113</v>
       </c>
@@ -3785,7 +5256,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="15" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>118</v>
       </c>
@@ -3793,7 +5264,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="15" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>116</v>
       </c>
@@ -3801,7 +5272,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="15" customHeight="1">
       <c r="A65" s="4" t="s">
         <v>117</v>
       </c>
@@ -3809,7 +5280,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="15" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>120</v>
       </c>
@@ -3817,7 +5288,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="15" customHeight="1">
       <c r="A67" s="7" t="s">
         <v>122</v>
       </c>
@@ -3825,7 +5296,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="15" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>124</v>
       </c>
@@ -3833,7 +5304,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="15" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>126</v>
       </c>
@@ -3841,7 +5312,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="15" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>129</v>
       </c>
@@ -3849,7 +5320,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="15" customHeight="1">
       <c r="A71" s="4" t="s">
         <v>130</v>
       </c>
@@ -3857,7 +5328,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="15" customHeight="1">
       <c r="A72" s="7" t="s">
         <v>132</v>
       </c>
@@ -3865,7 +5336,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="15" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>135</v>
       </c>
@@ -3873,7 +5344,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="15" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>137</v>
       </c>
@@ -3881,7 +5352,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" ht="15" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>138</v>
       </c>
@@ -3889,7 +5360,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" ht="15" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>139</v>
       </c>
@@ -3897,7 +5368,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" ht="15" customHeight="1">
       <c r="A77" s="4" t="s">
         <v>140</v>
       </c>
@@ -3905,7 +5376,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" ht="15" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>141</v>
       </c>
@@ -3913,7 +5384,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" ht="15" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>142</v>
       </c>
@@ -3921,7 +5392,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" ht="15" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>143</v>
       </c>
@@ -3929,7 +5400,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" ht="15" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>144</v>
       </c>
@@ -3937,7 +5408,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" ht="15" customHeight="1">
       <c r="A82" s="4" t="s">
         <v>145</v>
       </c>
@@ -3945,7 +5416,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" ht="15" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>146</v>
       </c>
@@ -3953,7 +5424,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" ht="15" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>147</v>
       </c>
@@ -3961,7 +5432,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" ht="15" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>148</v>
       </c>
@@ -3969,7 +5440,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" ht="15" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>149</v>
       </c>
@@ -3977,7 +5448,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" ht="15" customHeight="1">
       <c r="A87" s="4" t="s">
         <v>150</v>
       </c>
@@ -3985,7 +5456,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" ht="15" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>151</v>
       </c>
@@ -3993,7 +5464,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" ht="15" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>162</v>
       </c>
@@ -4001,7 +5472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" ht="15" customHeight="1">
       <c r="A90" s="4" t="s">
         <v>163</v>
       </c>
@@ -4009,7 +5480,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" ht="15" customHeight="1">
       <c r="A91" s="4" t="s">
         <v>164</v>
       </c>
@@ -4017,12 +5488,492 @@
         <v>164</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" ht="15" customHeight="1">
       <c r="A92" s="4" t="s">
         <v>165</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15" customHeight="1">
+      <c r="A93" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" customHeight="1">
+      <c r="A94" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" customHeight="1">
+      <c r="A95" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" customHeight="1">
+      <c r="A96" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" customHeight="1">
+      <c r="A97" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" customHeight="1">
+      <c r="A98" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15" customHeight="1">
+      <c r="A99" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15" customHeight="1">
+      <c r="A100" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15" customHeight="1">
+      <c r="A101" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15" customHeight="1">
+      <c r="A102" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15" customHeight="1">
+      <c r="A103" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15" customHeight="1">
+      <c r="A104" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15" customHeight="1">
+      <c r="A105" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15" customHeight="1">
+      <c r="A106" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" customHeight="1">
+      <c r="A107" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15" customHeight="1">
+      <c r="A108" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15" customHeight="1">
+      <c r="A109" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15" customHeight="1">
+      <c r="A110" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15" customHeight="1">
+      <c r="A111" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15" customHeight="1">
+      <c r="A112" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15" customHeight="1">
+      <c r="A113" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15" customHeight="1">
+      <c r="A114" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15" customHeight="1">
+      <c r="A115" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15" customHeight="1">
+      <c r="A116" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15" customHeight="1">
+      <c r="A117" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15" customHeight="1">
+      <c r="A118" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15" customHeight="1">
+      <c r="A119" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15" customHeight="1">
+      <c r="A120" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15" customHeight="1">
+      <c r="A121" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15" customHeight="1">
+      <c r="A122" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15" customHeight="1">
+      <c r="A123" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15" customHeight="1">
+      <c r="A124" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15" customHeight="1">
+      <c r="A125" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15" customHeight="1">
+      <c r="A126" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15" customHeight="1">
+      <c r="A127" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15" customHeight="1">
+      <c r="A128" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15" customHeight="1">
+      <c r="A129" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15" customHeight="1">
+      <c r="A130" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15" customHeight="1">
+      <c r="A131" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15" customHeight="1">
+      <c r="A132" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15" customHeight="1">
+      <c r="A133" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15" customHeight="1">
+      <c r="A134" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15" customHeight="1">
+      <c r="A135" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15" customHeight="1">
+      <c r="A136" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15" customHeight="1">
+      <c r="A137" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15" customHeight="1">
+      <c r="A138" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15" customHeight="1">
+      <c r="A139" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15" customHeight="1">
+      <c r="A140" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15" customHeight="1">
+      <c r="A141" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15" customHeight="1">
+      <c r="A142" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15" customHeight="1">
+      <c r="A143" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15" customHeight="1">
+      <c r="A144" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15" customHeight="1">
+      <c r="A145" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15" customHeight="1">
+      <c r="A146" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15" customHeight="1">
+      <c r="A147" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15" customHeight="1">
+      <c r="A148" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15" customHeight="1">
+      <c r="A149" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15" customHeight="1">
+      <c r="A150" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15" customHeight="1">
+      <c r="A151" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15" customHeight="1">
+      <c r="A152" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added detailed docstring and comments
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F860D9-EE59-4432-BAE2-28EDC65D346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59270F15-0AB1-49CD-A204-08B043228A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="403">
   <si>
     <t>exiobase</t>
   </si>
@@ -1161,6 +1161,81 @@
   </si>
   <si>
     <t>Wähle bis zu 3 Impacts zum Vergleichen aus.</t>
+  </si>
+  <si>
+    <t>Einstellungen öffnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Akzent </t>
+  </si>
+  <si>
+    <t>Dunkel 2</t>
+  </si>
+  <si>
+    <t>Open settings</t>
+  </si>
+  <si>
+    <t>Refresh</t>
+  </si>
+  <si>
+    <t>Export data</t>
+  </si>
+  <si>
+    <t>Aktualisieren</t>
+  </si>
+  <si>
+    <t>Daten exportieren</t>
+  </si>
+  <si>
+    <t>Impacts</t>
+  </si>
+  <si>
+    <t>Include units in column names</t>
+  </si>
+  <si>
+    <t>Einheiten in Spaltennamen aufnehmen</t>
+  </si>
+  <si>
+    <t>Localize column names</t>
+  </si>
+  <si>
+    <t>Output file</t>
+  </si>
+  <si>
+    <t>Excel Files (*.xlsx)</t>
+  </si>
+  <si>
+    <t>Please select at last one impact.</t>
+  </si>
+  <si>
+    <t>Please chose an .xlsx file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel export finished </t>
+  </si>
+  <si>
+    <t>Failed to export Excel</t>
+  </si>
+  <si>
+    <t>Fehler beim Excel-Export</t>
+  </si>
+  <si>
+    <t>Excel-Export abgeschlossen</t>
+  </si>
+  <si>
+    <t>Bitte eine .xlsx-Datei wählen.</t>
+  </si>
+  <si>
+    <t>Bitte mindestens einen Impact auswählen.</t>
+  </si>
+  <si>
+    <t>Excel-Dateien (*.xlsx)</t>
+  </si>
+  <si>
+    <t>Ausgabedatei</t>
+  </si>
+  <si>
+    <t>Spaltennamen lokalisieren</t>
   </si>
 </sst>
 </file>
@@ -2445,10 +2520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J167"/>
+  <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B167" sqref="B167"/>
+      <selection activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -3803,6 +3878,86 @@
         <v>376</v>
       </c>
     </row>
+    <row r="168" spans="1:2" ht="15" customHeight="1">
+      <c r="A168" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15" customHeight="1">
+      <c r="A169" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15" customHeight="1">
+      <c r="A170" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" customHeight="1">
+      <c r="A171" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" customHeight="1">
+      <c r="A172" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15" customHeight="1">
+      <c r="A173" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" customHeight="1">
+      <c r="A174" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15" customHeight="1">
+      <c r="A175" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15" customHeight="1">
+      <c r="A176" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" customHeight="1">
+      <c r="A177" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>395</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -3814,10 +3969,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B168"/>
+  <dimension ref="A1:B180"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173:A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -4993,7 +5148,7 @@
         <v>282</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>283</v>
+        <v>379</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15" customHeight="1">
@@ -5001,7 +5156,7 @@
         <v>284</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>285</v>
+        <v>380</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" customHeight="1">
@@ -5170,6 +5325,102 @@
       </c>
       <c r="B168" s="7" t="s">
         <v>377</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15" customHeight="1">
+      <c r="A169" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15" customHeight="1">
+      <c r="A170" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15" customHeight="1">
+      <c r="A171" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" customHeight="1">
+      <c r="A172" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15" customHeight="1">
+      <c r="A173" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" customHeight="1">
+      <c r="A174" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15" customHeight="1">
+      <c r="A175" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15" customHeight="1">
+      <c r="A176" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" customHeight="1">
+      <c r="A177" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15" customHeight="1">
+      <c r="A178" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15" customHeight="1">
+      <c r="A179" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" customHeight="1">
+      <c r="A180" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -5183,16 +5434,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="B171" sqref="B171"/>
+    <sheetView showGridLines="0" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174:B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="64" style="4" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="115" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -6563,6 +6814,86 @@
       </c>
       <c r="B171" s="7" t="s">
         <v>376</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15" customHeight="1">
+      <c r="A172" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15" customHeight="1">
+      <c r="A173" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15" customHeight="1">
+      <c r="A174" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15" customHeight="1">
+      <c r="A175" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15" customHeight="1">
+      <c r="A176" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15" customHeight="1">
+      <c r="A177" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15" customHeight="1">
+      <c r="A178" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15" customHeight="1">
+      <c r="A179" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15" customHeight="1">
+      <c r="A180" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15" customHeight="1">
+      <c r="A181" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Export to Excel function
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59270F15-0AB1-49CD-A204-08B043228A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D52434-DA18-4CC0-8CE1-8FAF5005BA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="404">
   <si>
     <t>exiobase</t>
   </si>
@@ -1184,9 +1184,6 @@
     <t>Aktualisieren</t>
   </si>
   <si>
-    <t>Daten exportieren</t>
-  </si>
-  <si>
     <t>Impacts</t>
   </si>
   <si>
@@ -1196,9 +1193,6 @@
     <t>Einheiten in Spaltennamen aufnehmen</t>
   </si>
   <si>
-    <t>Localize column names</t>
-  </si>
-  <si>
     <t>Output file</t>
   </si>
   <si>
@@ -1235,7 +1229,16 @@
     <t>Ausgabedatei</t>
   </si>
   <si>
-    <t>Spaltennamen lokalisieren</t>
+    <t>Choose impacts</t>
+  </si>
+  <si>
+    <t>Wähle Impacts aus</t>
+  </si>
+  <si>
+    <t>Excel export finished</t>
+  </si>
+  <si>
+    <t>Daten exportieren (Excel)</t>
   </si>
 </sst>
 </file>
@@ -2522,14 +2525,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B179" sqref="B179"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="60.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="115" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -3888,74 +3891,74 @@
     </row>
     <row r="169" spans="1:2" ht="15" customHeight="1">
       <c r="A169" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15" customHeight="1">
       <c r="A170" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" customHeight="1">
-      <c r="A171" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="B171" s="4" t="s">
-        <v>389</v>
+      <c r="A171" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" customHeight="1">
       <c r="A172" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -3971,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B180"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="A173" sqref="A173:A180"/>
+    <sheetView showGridLines="0" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A174" sqref="A174:XFD174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -5348,79 +5351,79 @@
         <v>383</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" customHeight="1">
       <c r="A172" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B173" s="4" t="s">
+    </row>
+    <row r="174" spans="1:2" ht="15" customHeight="1">
+      <c r="A174" s="7" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" ht="15" customHeight="1">
-      <c r="A174" s="4" t="s">
-        <v>389</v>
-      </c>
       <c r="B174" s="4" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="7" t="s">
-        <v>391</v>
-      </c>
-      <c r="B176" s="4" t="s">
-        <v>400</v>
+        <v>390</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="B177" s="7" t="s">
-        <v>399</v>
+        <v>391</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" customHeight="1">
       <c r="A178" s="7" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" customHeight="1">
       <c r="A179" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="B179" s="4" t="s">
         <v>394</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" customHeight="1">
       <c r="A180" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>396</v>
+        <v>400</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -5436,8 +5439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174:B181"/>
+    <sheetView showGridLines="0" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175:XFD175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
@@ -6826,74 +6829,74 @@
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
-      <c r="A175" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="B175" s="4" t="s">
-        <v>389</v>
+      <c r="A175" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" customHeight="1">
       <c r="A178" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" customHeight="1">
       <c r="A179" s="7" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" customHeight="1">
       <c r="A180" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" customHeight="1">
       <c r="A181" s="7" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Provided information about parameters in the advanced settings
</commit_message>
<xml_diff>
--- a/config/general.xlsx
+++ b/config/general.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\Hector\Kooperationsphase IO-Modelle\exiobase_explorer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D52434-DA18-4CC0-8CE1-8FAF5005BA41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D852A82-52E2-4100-9C52-494C83ABE1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exiobase" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="471">
   <si>
     <t>exiobase</t>
   </si>
@@ -500,9 +500,6 @@
     <t>Klassen (k)</t>
   </si>
   <si>
-    <t>Costum bins (kommagetrennt)</t>
-  </si>
-  <si>
     <t>Normalisierung (fließender Modus)</t>
   </si>
   <si>
@@ -1239,17 +1236,240 @@
   </si>
   <si>
     <t>Daten exportieren (Excel)</t>
+  </si>
+  <si>
+    <t>Continuous: Colors and legend use absolute values. Use Norm + Robust clipping + Gamma to control contrast.</t>
+  </si>
+  <si>
+    <t>Continuous: Farben und Legende basieren auf absoluten Werten. Kontrast über Normierung + Robustes Clipping + Gamma steuern.</t>
+  </si>
+  <si>
+    <t>Binned: Diskrete Klassen. Mit „Relativ“ klassifizierst Du nach Prozentanteilen (Summe = 100 %); sonst nach absoluten Werten.</t>
+  </si>
+  <si>
+    <t>Binned: Discrete classes. With 'Relative' you classify by percentage shares (sum = 100%); otherwise by absolute values.</t>
+  </si>
+  <si>
+    <t>Appearance</t>
+  </si>
+  <si>
+    <t>Darstellung</t>
+  </si>
+  <si>
+    <t>Binning (binned mode)</t>
+  </si>
+  <si>
+    <t>Klasseneinteilung (binned)</t>
+  </si>
+  <si>
+    <t>Relative</t>
+  </si>
+  <si>
+    <t>Relativ</t>
+  </si>
+  <si>
+    <t>Eigene Klassen (kommagetrennt)</t>
+  </si>
+  <si>
+    <t>Continuous scaling</t>
+  </si>
+  <si>
+    <t>Normierung</t>
+  </si>
+  <si>
+    <t>Robustes Clipping (%)</t>
+  </si>
+  <si>
+    <t>Gamma (Power-Norm)</t>
+  </si>
+  <si>
+    <t>Choose a color palette for the map.</t>
+  </si>
+  <si>
+    <t>Wähle eine Farbpalette für die Karte.</t>
+  </si>
+  <si>
+    <t>Invert the colormap.</t>
+  </si>
+  <si>
+    <t>Kehrt die Farbpalette um.</t>
+  </si>
+  <si>
+    <t>Show colorbar with value ranges.</t>
+  </si>
+  <si>
+    <t>Zeigt die Farbskala mit Wertebereichen an.</t>
+  </si>
+  <si>
+    <t>Optional title displayed above the map.</t>
+  </si>
+  <si>
+    <t>Optionaler Titel oberhalb der Karte.</t>
+  </si>
+  <si>
+    <t>Choose between binned (discrete classes) or continuous scale.</t>
+  </si>
+  <si>
+    <t>If checked, classes use percentage shares (sum=100%). If unchecked, absolute values.</t>
+  </si>
+  <si>
+    <t>Wenn aktiv, werden Klassen nach Anteilen in Prozent (Summe=100 %) gebildet; sonst nach absoluten Werten.</t>
+  </si>
+  <si>
+    <t>Number of classes when no custom bins are provided.</t>
+  </si>
+  <si>
+    <t>Anzahl der Klassen, wenn keine eigenen Grenzen angegeben sind.</t>
+  </si>
+  <si>
+    <t>Comma-separated inner class boundaries. dmin and dmax are added automatically.</t>
+  </si>
+  <si>
+    <t>Kommagetrennte innere Klassengrenzen. Minimum und Maximum werden automatisch ergänzt.</t>
+  </si>
+  <si>
+    <t>Quantile clipping for vmin/vmax (e.g., 2% uses 2nd and 98th percentiles).</t>
+  </si>
+  <si>
+    <t>Bestimmt vmin/vmax über Quantile (z. B. 2 % nutzt 2. und 98. Perzentil).</t>
+  </si>
+  <si>
+    <t>PowerNorm exponent: &lt;1 enhances small values, &gt;1 enhances large values.</t>
+  </si>
+  <si>
+    <t>Exponent für PowerNorm: &lt;1 betont kleine Werte, &gt;1 betont große Werte.</t>
+  </si>
+  <si>
+    <t>Colormap used to color the countries. Use 'Reverse' to invert light/dark order.</t>
+  </si>
+  <si>
+    <t>Farbpalette zur Einfärbung der Länder. Mit „Umkehren“ wird die Hell/Dunkel-Reihenfolge invertiert.</t>
+  </si>
+  <si>
+    <t>Inverts the selected colormap.</t>
+  </si>
+  <si>
+    <t>Invertiert die gewählte Farbpalette.</t>
+  </si>
+  <si>
+    <t>Displays a legend. In continuous mode it shows absolute values; in binned mode it shows numeric ranges per class.</t>
+  </si>
+  <si>
+    <t>Blendet eine Legende ein. Im Modus „continuous“ zeigt sie absolute Werte, im Modus „binned“ numerische Klassenbereiche.</t>
+  </si>
+  <si>
+    <t>Optional title for the map.</t>
+  </si>
+  <si>
+    <t>Optionaler Titel für die Karte.</t>
+  </si>
+  <si>
+    <t>continuous: Colors reflect absolute values with a continuous legend.
+binned: Discrete classes. With 'Relative' you bin by percentage shares.</t>
+  </si>
+  <si>
+    <t>continuous: Farben spiegeln absolute Werte wider, die Legende ist stetig.
+binned: Diskrete Klassen. Mit „Relativ“ erfolgt die Einteilung nach Prozentanteilen.</t>
+  </si>
+  <si>
+    <t>Binned mode only: toggle between absolute values and percentage shares for the class breaks.</t>
+  </si>
+  <si>
+    <t>Nur im binned-Modus: Umschalten zwischen absoluten Werten und Prozentanteilen für die Klassengrenzen.</t>
+  </si>
+  <si>
+    <t>Number of discrete classes. If 'Custom bins' are provided, they take precedence.</t>
+  </si>
+  <si>
+    <t>Anzahl der diskreten Klassen. Bei „Eigene Klassen“ haben diese Vorrang.</t>
+  </si>
+  <si>
+    <t>Enter inner edges like '10, 25, 50'. The dialog will prepend the data minimum and append the maximum.</t>
+  </si>
+  <si>
+    <t>Innere Kanten eingeben, z. B. „10, 25, 50“. Minimum und Maximum werden automatisch ergänzt.</t>
+  </si>
+  <si>
+    <t>Normalization for continuous mode:
+- linear: uniform mapping from vmin..vmax
+- log: logarithmic mapping; requires strictly positive values
+- power: Power-law mapping; see Gamma</t>
+  </si>
+  <si>
+    <t>Normierung für den continuous-Modus:
+- linear: gleichmäßige Abbildung von vmin..vmax
+- log: logarithmische Abbildung; nur für strikt positive Werte
+- power: Potenz-Abbildung; siehe Gamma</t>
+  </si>
+  <si>
+    <t>Robust clipping determines vmin/vmax from quantiles instead of absolute min/max to reduce outlier effects.</t>
+  </si>
+  <si>
+    <t>Robustes Clipping bestimmt vmin/vmax über Quantile statt über Min/Max, um Ausreißer zu dämpfen.</t>
+  </si>
+  <si>
+    <t>Gamma (PowerNorm):
+- gamma &lt; 1 emphasises lower value range
+- gamma &gt; 1 emphasises higher value range</t>
+  </si>
+  <si>
+    <t>Gamma (PowerNorm):
+- gamma &lt; 1 betont den unteren Wertebereich
+- gamma &gt; 1 betont den oberen Wertebereich</t>
+  </si>
+  <si>
+    <t>Linear: uniform color steps from vmin to vmax.</t>
+  </si>
+  <si>
+    <t>Linear: gleichmäßige Farbabstufung von vmin bis vmax.</t>
+  </si>
+  <si>
+    <t>Log: emphasises orders of magnitude; requires strictly positive data.</t>
+  </si>
+  <si>
+    <t>Log: betont Größenordnungen; erfordert strikt positive Daten.</t>
+  </si>
+  <si>
+    <t>Power: adjust contrast with Gamma (&lt;1: highlights small values; &gt;1: highlights large).</t>
+  </si>
+  <si>
+    <t>Power: Kontrast über Gamma steuern (&lt;1: betont kleine Werte; &gt;1: betont große).</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Hilfe</t>
+  </si>
+  <si>
+    <t>Wähle zwischen diskreten Klassen (binned) und stetiger Skala (continuous).</t>
+  </si>
+  <si>
+    <t>linear: uniform steps | log: highlight orders of magnitude (logarithmic) | power: adjustable contrast with gamma</t>
+  </si>
+  <si>
+    <t>linear: gleichmäßige Schritte | log: betont Größenordnungen (logarithmisch) | power: anpassbarer Kontrast mit Gamma</t>
+  </si>
+  <si>
+    <t>Stetige Skalierung (continuous)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1340,32 +1560,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{C2F78208-F7F8-4542-9E5B-6270DCB86735}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{C71F7E32-9819-48E7-8142-C8147DEC96B1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -2525,7 +2747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A148" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A148" workbookViewId="0">
       <selection activeCell="A176" sqref="A176"/>
     </sheetView>
   </sheetViews>
@@ -3219,58 +3441,58 @@
     </row>
     <row r="85" spans="1:2" ht="15" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15" customHeight="1">
@@ -3283,682 +3505,682 @@
     </row>
     <row r="93" spans="1:2" ht="15" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15" customHeight="1">
       <c r="A95" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15" customHeight="1">
       <c r="A96" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B141" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" customHeight="1">
       <c r="A142" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B142" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" customHeight="1">
       <c r="A143" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" customHeight="1">
       <c r="A144" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B144" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" customHeight="1">
       <c r="A145" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" customHeight="1">
       <c r="A146" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15" customHeight="1">
       <c r="A147" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" customHeight="1">
       <c r="A148" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15" customHeight="1">
       <c r="A149" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" customHeight="1">
       <c r="A150" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15" customHeight="1">
       <c r="A151" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15" customHeight="1">
       <c r="A152" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15" customHeight="1">
       <c r="A153" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15" customHeight="1">
       <c r="A154" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15" customHeight="1">
       <c r="A155" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15" customHeight="1">
       <c r="A156" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15" customHeight="1">
       <c r="A157" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15" customHeight="1">
       <c r="A158" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15" customHeight="1">
       <c r="A159" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15" customHeight="1">
       <c r="A160" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" customHeight="1">
       <c r="A161" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15" customHeight="1">
       <c r="A162" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15" customHeight="1">
       <c r="A163" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" customHeight="1">
       <c r="A164" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" customHeight="1">
       <c r="A165" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" customHeight="1">
       <c r="A166" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15" customHeight="1">
       <c r="A167" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15" customHeight="1">
       <c r="A168" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15" customHeight="1">
       <c r="A169" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15" customHeight="1">
       <c r="A170" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" customHeight="1">
       <c r="A171" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" customHeight="1">
       <c r="A172" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -3972,16 +4194,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B180"/>
+  <dimension ref="A1:B213"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174:XFD174"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="B188" sqref="B188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="54.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="67" style="4" customWidth="1"/>
+    <col min="2" max="2" width="62" style="4" customWidth="1"/>
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -4551,7 +4773,7 @@
         <v>138</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15" customHeight="1">
@@ -4599,7 +4821,7 @@
         <v>144</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>157</v>
+        <v>413</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15" customHeight="1">
@@ -4607,7 +4829,7 @@
         <v>145</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15" customHeight="1">
@@ -4631,7 +4853,7 @@
         <v>148</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15" customHeight="1">
@@ -4639,7 +4861,7 @@
         <v>149</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15" customHeight="1">
@@ -4647,7 +4869,7 @@
         <v>150</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>150</v>
+        <v>416</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15" customHeight="1">
@@ -4655,63 +4877,63 @@
         <v>151</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>151</v>
+        <v>417</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15" customHeight="1">
       <c r="A85" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15" customHeight="1">
       <c r="A86" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15" customHeight="1">
       <c r="A87" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15" customHeight="1">
       <c r="A88" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" customHeight="1">
       <c r="A91" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>174</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15" customHeight="1">
@@ -4719,711 +4941,975 @@
         <v>135</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" customHeight="1">
       <c r="A93" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B93" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15" customHeight="1">
       <c r="A94" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B94" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15" customHeight="1">
       <c r="A95" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15" customHeight="1">
       <c r="A96" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15" customHeight="1">
       <c r="A97" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15" customHeight="1">
       <c r="A98" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15" customHeight="1">
       <c r="A99" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15" customHeight="1">
       <c r="A100" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B100" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" customHeight="1">
       <c r="A101" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>192</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15" customHeight="1">
       <c r="A102" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15" customHeight="1">
       <c r="A103" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15" customHeight="1">
       <c r="A104" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15" customHeight="1">
       <c r="A105" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15" customHeight="1">
       <c r="A106" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>202</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>204</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B108" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B110" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B112" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B113" s="4" t="s">
         <v>216</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B114" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B115" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="B116" s="4" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B117" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="B117" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B118" s="4" t="s">
         <v>226</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B119" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>230</v>
-      </c>
-      <c r="B120" s="4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B122" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B124" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B125" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B127" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B128" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B129" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="B129" s="4" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B130" s="4" t="s">
         <v>250</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B131" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>254</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B133" s="4" t="s">
         <v>256</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B134" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="B134" s="4" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B135" s="4" t="s">
         <v>260</v>
-      </c>
-      <c r="B135" s="4" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B136" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B137" s="4" t="s">
         <v>264</v>
-      </c>
-      <c r="B137" s="4" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B138" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B139" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B140" s="4" t="s">
         <v>270</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B141" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="B141" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" customHeight="1">
       <c r="A142" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B142" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" customHeight="1">
       <c r="A143" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" customHeight="1">
       <c r="A144" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B144" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="B144" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" customHeight="1">
       <c r="A145" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" customHeight="1">
       <c r="A146" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15" customHeight="1">
       <c r="A147" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" customHeight="1">
       <c r="A148" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15" customHeight="1">
       <c r="A149" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B149" s="7" t="s">
         <v>337</v>
-      </c>
-      <c r="B149" s="7" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" customHeight="1">
       <c r="A150" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15" customHeight="1">
       <c r="A151" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="B151" s="7" t="s">
         <v>340</v>
-      </c>
-      <c r="B151" s="7" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15" customHeight="1">
       <c r="A152" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B152" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15" customHeight="1">
       <c r="A153" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="B153" s="7" t="s">
         <v>344</v>
-      </c>
-      <c r="B153" s="7" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15" customHeight="1">
       <c r="A154" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="B154" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="B154" s="7" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15" customHeight="1">
       <c r="A155" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B155" s="7" t="s">
         <v>348</v>
-      </c>
-      <c r="B155" s="7" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15" customHeight="1">
       <c r="A156" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B156" s="7" t="s">
         <v>350</v>
-      </c>
-      <c r="B156" s="7" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15" customHeight="1">
       <c r="A157" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B157" s="7" t="s">
         <v>352</v>
-      </c>
-      <c r="B157" s="7" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15" customHeight="1">
       <c r="A158" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="B158" s="7" t="s">
         <v>354</v>
-      </c>
-      <c r="B158" s="7" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15" customHeight="1">
       <c r="A159" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B159" s="7" t="s">
         <v>357</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15" customHeight="1">
       <c r="A160" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B160" s="7" t="s">
         <v>359</v>
-      </c>
-      <c r="B160" s="7" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" customHeight="1">
       <c r="A161" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B161" s="7" t="s">
         <v>361</v>
-      </c>
-      <c r="B161" s="7" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15" customHeight="1">
       <c r="A162" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>363</v>
-      </c>
-      <c r="B162" s="7" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15" customHeight="1">
       <c r="A163" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="B163" s="7" t="s">
         <v>365</v>
-      </c>
-      <c r="B163" s="7" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" customHeight="1">
       <c r="A164" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" customHeight="1">
       <c r="A165" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" customHeight="1">
       <c r="A166" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15" customHeight="1">
       <c r="A167" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B167" s="7" t="s">
         <v>374</v>
-      </c>
-      <c r="B167" s="7" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15" customHeight="1">
       <c r="A168" s="7" t="s">
+        <v>375</v>
+      </c>
+      <c r="B168" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="B168" s="7" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15" customHeight="1">
       <c r="A169" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15" customHeight="1">
       <c r="A170" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" customHeight="1">
       <c r="A171" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" customHeight="1">
       <c r="A172" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B173" s="4" t="s">
         <v>386</v>
-      </c>
-      <c r="B173" s="4" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" customHeight="1">
       <c r="A178" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" customHeight="1">
       <c r="A179" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="B179" s="4" t="s">
         <v>393</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" customHeight="1">
       <c r="A180" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="B180" s="7" t="s">
         <v>400</v>
       </c>
-      <c r="B180" s="7" t="s">
-        <v>401</v>
+    </row>
+    <row r="181" spans="1:2" ht="15" customHeight="1">
+      <c r="A181" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15" customHeight="1">
+      <c r="A182" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15" customHeight="1">
+      <c r="A183" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15" customHeight="1">
+      <c r="A184" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15" customHeight="1">
+      <c r="A185" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B185" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15" customHeight="1">
+      <c r="A186" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15" customHeight="1">
+      <c r="A187" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15" customHeight="1">
+      <c r="A188" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15" customHeight="1">
+      <c r="A189" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15" customHeight="1">
+      <c r="A190" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15" customHeight="1">
+      <c r="A191" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="15" customHeight="1">
+      <c r="A192" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15" customHeight="1">
+      <c r="A193" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15" customHeight="1">
+      <c r="A194" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15" customHeight="1">
+      <c r="A195" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15" customHeight="1">
+      <c r="A196" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15" customHeight="1">
+      <c r="A197" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15" customHeight="1">
+      <c r="A198" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15" customHeight="1">
+      <c r="A199" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15" customHeight="1">
+      <c r="A200" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15" customHeight="1">
+      <c r="A201" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15" customHeight="1">
+      <c r="A202" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="15" customHeight="1">
+      <c r="A203" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="15" customHeight="1">
+      <c r="A204" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15" customHeight="1">
+      <c r="A205" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="15" customHeight="1">
+      <c r="A206" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="15" customHeight="1">
+      <c r="A207" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="15" customHeight="1">
+      <c r="A208" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="15" customHeight="1">
+      <c r="A209" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="15" customHeight="1">
+      <c r="A210" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="15" customHeight="1">
+      <c r="A211" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="15" customHeight="1">
+      <c r="A212" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="15" customHeight="1">
+      <c r="A213" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -6157,58 +6643,58 @@
     </row>
     <row r="89" spans="1:2" ht="15" customHeight="1">
       <c r="A89" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15" customHeight="1">
       <c r="A90" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15" customHeight="1">
       <c r="A91" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15" customHeight="1">
       <c r="A92" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15" customHeight="1">
       <c r="A93" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15" customHeight="1">
       <c r="A94" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15" customHeight="1">
       <c r="A95" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15" customHeight="1">
@@ -6221,682 +6707,682 @@
     </row>
     <row r="97" spans="1:2" ht="15" customHeight="1">
       <c r="A97" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15" customHeight="1">
       <c r="A98" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15" customHeight="1">
       <c r="A99" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15" customHeight="1">
       <c r="A100" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15" customHeight="1">
       <c r="A101" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15" customHeight="1">
       <c r="A102" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15" customHeight="1">
       <c r="A103" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15" customHeight="1">
       <c r="A104" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15" customHeight="1">
       <c r="A105" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15" customHeight="1">
       <c r="A106" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15" customHeight="1">
       <c r="A107" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15" customHeight="1">
       <c r="A108" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15" customHeight="1">
       <c r="A109" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15" customHeight="1">
       <c r="A110" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15" customHeight="1">
       <c r="A111" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15" customHeight="1">
       <c r="A112" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15" customHeight="1">
       <c r="A113" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:2" ht="15" customHeight="1">
       <c r="A114" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15" customHeight="1">
       <c r="A115" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15" customHeight="1">
       <c r="A116" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="15" customHeight="1">
       <c r="A117" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="118" spans="1:2" ht="15" customHeight="1">
       <c r="A118" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="119" spans="1:2" ht="15" customHeight="1">
       <c r="A119" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="120" spans="1:2" ht="15" customHeight="1">
       <c r="A120" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="15" customHeight="1">
       <c r="A121" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15" customHeight="1">
       <c r="A122" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15" customHeight="1">
       <c r="A123" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15" customHeight="1">
       <c r="A124" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="15" customHeight="1">
       <c r="A125" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15" customHeight="1">
       <c r="A126" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15" customHeight="1">
       <c r="A127" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15" customHeight="1">
       <c r="A128" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="129" spans="1:2" ht="15" customHeight="1">
       <c r="A129" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15" customHeight="1">
       <c r="A130" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15" customHeight="1">
       <c r="A131" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="132" spans="1:2" ht="15" customHeight="1">
       <c r="A132" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15" customHeight="1">
       <c r="A133" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15" customHeight="1">
       <c r="A134" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15" customHeight="1">
       <c r="A135" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15" customHeight="1">
       <c r="A136" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15" customHeight="1">
       <c r="A137" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15" customHeight="1">
       <c r="A138" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15" customHeight="1">
       <c r="A139" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15" customHeight="1">
       <c r="A140" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15" customHeight="1">
       <c r="A141" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="15" customHeight="1">
       <c r="A142" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15" customHeight="1">
       <c r="A143" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="144" spans="1:2" ht="15" customHeight="1">
       <c r="A144" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15" customHeight="1">
       <c r="A145" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B145" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15" customHeight="1">
       <c r="A146" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B146" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="B146" s="4" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="15" customHeight="1">
       <c r="A147" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B147" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="B147" s="4" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15" customHeight="1">
       <c r="A148" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B148" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15" customHeight="1">
       <c r="A149" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B149" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="B149" s="4" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15" customHeight="1">
       <c r="A150" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B150" s="4" t="s">
         <v>282</v>
-      </c>
-      <c r="B150" s="4" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15" customHeight="1">
       <c r="A151" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B151" s="4" t="s">
         <v>284</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15" customHeight="1">
       <c r="A152" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B152" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="B152" s="4" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15" customHeight="1">
       <c r="A153" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="15" customHeight="1">
       <c r="A154" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15" customHeight="1">
       <c r="A155" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="156" spans="1:2" ht="15" customHeight="1">
       <c r="A156" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B156" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="15" customHeight="1">
       <c r="A157" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="158" spans="1:2" ht="15" customHeight="1">
       <c r="A158" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B158" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15" customHeight="1">
       <c r="A159" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15" customHeight="1">
       <c r="A160" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="161" spans="1:2" ht="15" customHeight="1">
       <c r="A161" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="162" spans="1:2" ht="15" customHeight="1">
       <c r="A162" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15" customHeight="1">
       <c r="A163" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15" customHeight="1">
       <c r="A164" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15" customHeight="1">
       <c r="A165" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B165" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15" customHeight="1">
       <c r="A166" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B166" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15" customHeight="1">
       <c r="A167" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="168" spans="1:2" ht="15" customHeight="1">
       <c r="A168" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="169" spans="1:2" ht="15" customHeight="1">
       <c r="A169" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="170" spans="1:2" ht="15" customHeight="1">
       <c r="A170" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="171" spans="1:2" ht="15" customHeight="1">
       <c r="A171" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="172" spans="1:2" ht="15" customHeight="1">
       <c r="A172" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15" customHeight="1">
       <c r="A173" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15" customHeight="1">
       <c r="A174" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15" customHeight="1">
       <c r="A175" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15" customHeight="1">
       <c r="A176" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B176" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="177" spans="1:2" ht="15" customHeight="1">
       <c r="A177" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15" customHeight="1">
       <c r="A178" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15" customHeight="1">
       <c r="A179" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="180" spans="1:2" ht="15" customHeight="1">
       <c r="A180" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="181" spans="1:2" ht="15" customHeight="1">
       <c r="A181" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>